<commit_message>
added dataprovider utils for test iteration
</commit_message>
<xml_diff>
--- a/src/main/java/com/framework/TestData/testConfig.xlsx
+++ b/src/main/java/com/framework/TestData/testConfig.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RunManager" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -53,6 +54,36 @@
   </si>
   <si>
     <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mini bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newTest</t>
   </si>
 </sst>
 </file>
@@ -62,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,6 +114,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,12 +165,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,11 +197,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -212,4 +254,119 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="admin@123"/>
+    <hyperlink ref="D3" r:id="rId2" display="admin@123"/>
+    <hyperlink ref="D4" r:id="rId3" display="admin@123"/>
+    <hyperlink ref="D5" r:id="rId4" display="admin@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added data provider test exceution and util
</commit_message>
<xml_diff>
--- a/src/main/java/com/framework/TestData/testConfig.xlsx
+++ b/src/main/java/com/framework/TestData/testConfig.xlsx
@@ -68,7 +68,7 @@
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">admin@123</t>
+    <t xml:space="preserve">admin123</t>
   </si>
   <si>
     <t xml:space="preserve">rajesh</t>
@@ -93,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,13 +114,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,16 +158,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,7 +190,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -264,10 +253,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -276,13 +265,13 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -293,13 +282,13 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -310,13 +299,13 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -324,43 +313,37 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="admin@123"/>
-    <hyperlink ref="D3" r:id="rId2" display="admin@123"/>
-    <hyperlink ref="D4" r:id="rId3" display="admin@123"/>
-    <hyperlink ref="D5" r:id="rId4" display="admin@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added browser support from excel for each tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/framework/TestData/testConfig.xlsx
+++ b/src/main/java/com/framework/TestData/testConfig.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t xml:space="preserve">testname</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
+    <t xml:space="preserve">browser</t>
+  </si>
+  <si>
     <t xml:space="preserve">username</t>
   </si>
   <si>
@@ -65,6 +68,9 @@
     <t xml:space="preserve">fname</t>
   </si>
   <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
@@ -72,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">rajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firefox</t>
   </si>
   <si>
     <t xml:space="preserve">mini bytes</t>
@@ -250,10 +259,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,6 +283,9 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -283,13 +295,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,13 +315,16 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,30 +335,36 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Custom Exceptions and remvoed exceptions
</commit_message>
<xml_diff>
--- a/src/main/java/com/framework/TestData/testConfig.xlsx
+++ b/src/main/java/com/framework/TestData/testConfig.xlsx
@@ -199,7 +199,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="20.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -262,10 +262,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -355,7 +355,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>

</xml_diff>